<commit_message>
LITE-28561 Implement sync PPR to marketplaces
</commit_message>
<xml_diff>
--- a/tests/fixtures/test_PPR_file_delegate_l2.xlsx
+++ b/tests/fixtures/test_PPR_file_delegate_l2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/igrebenshikov00/GIT/connect-extension-xvs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/igrebenshikov00/GIT/connect-extension-xvs/tests/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{842629FD-6D56-9947-9F11-22911264FDA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2596981-CB8A-8444-AB36-9B30F03F69D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17400" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="201">
   <si>
     <t>Name_EN</t>
   </si>
@@ -5169,8 +5169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BL45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BE1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="BI8" sqref="BI8"/>
+    <sheetView tabSelected="1" topLeftCell="AD1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AH7" sqref="AH7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="29.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5804,8 +5804,8 @@
       <c r="AF4" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="AG4" s="3" t="s">
-        <v>182</v>
+      <c r="AG4" s="3" t="b">
+        <v>0</v>
       </c>
       <c r="AH4" s="3" t="s">
         <v>182</v>
@@ -5981,8 +5981,8 @@
       <c r="AG5" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="AH5" s="3" t="s">
-        <v>182</v>
+      <c r="AH5" s="3" t="b">
+        <v>0</v>
       </c>
       <c r="AI5" s="3" t="s">
         <v>182</v>
@@ -6155,8 +6155,8 @@
       <c r="AG6" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="AH6" s="3" t="s">
-        <v>182</v>
+      <c r="AH6" s="3" t="b">
+        <v>0</v>
       </c>
       <c r="AI6" s="3" t="s">
         <v>182</v>

</xml_diff>